<commit_message>
updated location of tables and curb in two scenes
</commit_message>
<xml_diff>
--- a/Map/tables_XY.xlsx
+++ b/Map/tables_XY.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="8">
   <si>
     <t>1_1_2</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>1_2_2</t>
-  </si>
-  <si>
-    <t>L2</t>
   </si>
   <si>
     <t>L1</t>
@@ -369,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +396,7 @@
         <v>48.816546608259301</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -413,7 +410,7 @@
         <v>42.210640178163302</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -427,7 +424,7 @@
         <v>42.7933982445686</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -441,7 +438,7 @@
         <v>49.305788005875897</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -455,7 +452,7 @@
         <v>50.833557637082102</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -469,7 +466,7 @@
         <v>40.146702285215397</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -477,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>20.506374249881599</v>
+        <v>22.253234658833499</v>
       </c>
       <c r="C8">
-        <v>50.877619183289099</v>
+        <v>51.924517584393101</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -491,13 +488,13 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>26.618290369901001</v>
+        <v>31.8379873340808</v>
       </c>
       <c r="C9">
-        <v>44.864782173648898</v>
+        <v>45.558545389720301</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -505,13 +502,13 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>31.231986692311999</v>
+        <v>32.202688219478901</v>
       </c>
       <c r="C10">
-        <v>47.4618234929995</v>
+        <v>46.641217335449902</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -519,40 +516,155 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>23.853540205384999</v>
+        <v>23.098798093478699</v>
       </c>
       <c r="C11">
-        <v>52.556390198728899</v>
+        <v>52.277863776413199</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>17.649968001206801</v>
-      </c>
-      <c r="C12">
-        <v>50.983547212079799</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B13">
+        <v>20.506374249881599</v>
+      </c>
+      <c r="C13">
+        <v>50.877619183289099</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>26.618290369901001</v>
+      </c>
+      <c r="C14">
+        <v>44.864782173648898</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>31.231986692311999</v>
+      </c>
+      <c r="C15">
+        <v>47.4618234929995</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>23.853540205384999</v>
+      </c>
+      <c r="C16">
+        <v>52.556390198728899</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>20.74489693192</v>
+      </c>
+      <c r="C17">
+        <v>50.989183559230199</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>27.079077645497499</v>
+      </c>
+      <c r="C18">
+        <v>44.804069782875501</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>32.1683532398525</v>
+      </c>
+      <c r="C19">
+        <v>47.484351615978099</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>24.560590385063598</v>
+      </c>
+      <c r="C20">
+        <v>52.644645299068102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>17.649968001206801</v>
+      </c>
+      <c r="C21">
+        <v>50.983547212079799</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
         <v>26.604417284489902</v>
       </c>
-      <c r="C13">
+      <c r="C22">
         <v>41.826861947842303</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D22" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated table locations and curb
</commit_message>
<xml_diff>
--- a/Map/tables_XY.xlsx
+++ b/Map/tables_XY.xlsx
@@ -368,8 +368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
complete tables' locations for all scene
</commit_message>
<xml_diff>
--- a/Map/tables_XY.xlsx
+++ b/Map/tables_XY.xlsx
@@ -14,6 +14,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">17</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="21">
   <si>
     <t>1_1_2</t>
   </si>
@@ -54,6 +58,39 @@
   </si>
   <si>
     <t>code</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>1_2_1</t>
+  </si>
+  <si>
+    <t>1_4_2</t>
+  </si>
+  <si>
+    <t>1_5_2</t>
+  </si>
+  <si>
+    <t>1_6_2</t>
+  </si>
+  <si>
+    <t>1_6_1</t>
+  </si>
+  <si>
+    <t>1_7_2</t>
+  </si>
+  <si>
+    <t>1_7_1</t>
+  </si>
+  <si>
+    <t>1_8_2</t>
+  </si>
+  <si>
+    <t>1_9_1</t>
+  </si>
+  <si>
+    <t>1_9_2</t>
   </si>
 </sst>
 </file>
@@ -372,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,6 +447,9 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -424,6 +464,9 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
+      <c r="E3">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -438,6 +481,9 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
+      <c r="E4">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -452,19 +498,25 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
+      <c r="E5">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6">
-        <v>17.340371911653602</v>
+        <v>16.544686205524599</v>
       </c>
       <c r="C6">
-        <v>50.833557637082102</v>
+        <v>51.644702488902901</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
+      </c>
+      <c r="E6">
+        <v>14.2736</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -472,18 +524,21 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>28.4417177573347</v>
+        <v>29.3052736869241</v>
       </c>
       <c r="C7">
-        <v>40.146702285215397</v>
+        <v>39.321205934378</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
+      <c r="E7">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <v>22.253234658833499</v>
@@ -494,10 +549,13 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
+      <c r="E8">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>31.8379873340808</v>
@@ -508,10 +566,13 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
+      <c r="E9">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B10">
         <v>32.202688219478901</v>
@@ -522,10 +583,13 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
+      <c r="E10">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>23.098798093478699</v>
@@ -536,151 +600,2042 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
+      <c r="E11">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>17.754119656157599</v>
+      </c>
+      <c r="C12">
+        <v>43.039246825301099</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>14.2736</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>20.506374249881599</v>
+        <v>19.495225339373299</v>
       </c>
       <c r="C13">
-        <v>50.877619183289099</v>
+        <v>44.804300055269699</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>14.2736</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>26.618290369901001</v>
+        <v>25.300288199900798</v>
       </c>
       <c r="C14">
-        <v>44.864782173648898</v>
+        <v>40.405637538060098</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>14.2736</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>22.637478122253299</v>
+      </c>
+      <c r="C15">
+        <v>38.614118420576602</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>20.050742392421</v>
+      </c>
+      <c r="C17">
+        <v>51.460772519751302</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>28.633606244981198</v>
+      </c>
+      <c r="C18">
+        <v>43.750133457742898</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>33.648982120948801</v>
+      </c>
+      <c r="C19">
+        <v>45.357271110573997</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>23.3736469565543</v>
+      </c>
+      <c r="C20">
+        <v>52.812204722589698</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>17.2167058082014</v>
+      </c>
+      <c r="C21">
+        <v>43.3058923721524</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>19.5356816464001</v>
+      </c>
+      <c r="C22">
+        <v>45.003379975785599</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>25.145022019760201</v>
+      </c>
+      <c r="C23">
+        <v>40.279519204107501</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>21.674027202388402</v>
+      </c>
+      <c r="C24">
+        <v>38.641865651372697</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>17.8702774327535</v>
+      </c>
+      <c r="C25">
+        <v>50.884222231472201</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>27.084533342256599</v>
+      </c>
+      <c r="C26">
+        <v>41.642812540765398</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15">
+      <c r="B29">
+        <v>20.506374249881599</v>
+      </c>
+      <c r="C29">
+        <v>50.877619183289099</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>26.618290369901001</v>
+      </c>
+      <c r="C30">
+        <v>44.864782173648898</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
         <v>31.231986692311999</v>
       </c>
-      <c r="C15">
+      <c r="C31">
         <v>47.4618234929995</v>
       </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16">
+      <c r="B32">
         <v>23.853540205384999</v>
       </c>
-      <c r="C16">
+      <c r="C32">
         <v>52.556390198728899</v>
       </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17">
+      <c r="B33">
         <v>20.74489693192</v>
       </c>
-      <c r="C17">
+      <c r="C33">
         <v>50.989183559230199</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="E33">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B34">
         <v>27.079077645497499</v>
       </c>
-      <c r="C18">
+      <c r="C34">
         <v>44.804069782875501</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="E34">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19">
+      <c r="B35">
         <v>32.1683532398525</v>
       </c>
-      <c r="C19">
+      <c r="C35">
         <v>47.484351615978099</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D35" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="E35">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20">
+      <c r="B36">
         <v>24.560590385063598</v>
       </c>
-      <c r="C20">
+      <c r="C36">
         <v>52.644645299068102</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="E36">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21">
-        <v>17.649968001206801</v>
-      </c>
-      <c r="C21">
-        <v>50.983547212079799</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B37">
+        <v>16.7812655621535</v>
+      </c>
+      <c r="C37">
+        <v>51.932146167890899</v>
+      </c>
+      <c r="D37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="E37">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22">
-        <v>26.604417284489902</v>
-      </c>
-      <c r="C22">
-        <v>41.826861947842303</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B38">
+        <v>27.8598107566661</v>
+      </c>
+      <c r="C38">
+        <v>40.889504474261699</v>
+      </c>
+      <c r="D38" t="s">
         <v>5</v>
       </c>
+      <c r="E38">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>17.384425129982201</v>
+      </c>
+      <c r="C39">
+        <v>43.116890174588299</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>19.588925656439901</v>
+      </c>
+      <c r="C40">
+        <v>44.977625042219302</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>24.807841496589798</v>
+      </c>
+      <c r="C41">
+        <v>40.759934026461899</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>21.239188434820399</v>
+      </c>
+      <c r="C42">
+        <v>39.006405461680899</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>21.4278541376849</v>
+      </c>
+      <c r="C44">
+        <v>50.729102765604999</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>30.374630227260301</v>
+      </c>
+      <c r="C45">
+        <v>41.858414031402603</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>36.141410988547896</v>
+      </c>
+      <c r="C46">
+        <v>42.856720789482502</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>24.107748358881501</v>
+      </c>
+      <c r="C47">
+        <v>52.3968862062856</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>16.8946769678561</v>
+      </c>
+      <c r="C48">
+        <v>43.066860244882101</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <v>18.871602809527801</v>
+      </c>
+      <c r="C49">
+        <v>44.666789739271401</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50">
+        <v>25.452039875349801</v>
+      </c>
+      <c r="C50">
+        <v>40.606541398145801</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51">
+        <v>21.659301240428199</v>
+      </c>
+      <c r="C51">
+        <v>39.008875558070002</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52">
+        <v>16.313209629610501</v>
+      </c>
+      <c r="C52">
+        <v>51.707379022406897</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53">
+        <v>30.183480835146</v>
+      </c>
+      <c r="C53">
+        <v>38.7902775051069</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55">
+        <v>23.707262528731</v>
+      </c>
+      <c r="C55">
+        <v>52.648478210130598</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56">
+        <v>21.183812840628999</v>
+      </c>
+      <c r="C56">
+        <v>51.675378719740102</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57">
+        <v>34.313298875221399</v>
+      </c>
+      <c r="C57">
+        <v>41.052207997657803</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58">
+        <v>36.424072681287299</v>
+      </c>
+      <c r="C58">
+        <v>42.144354221438299</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59">
+        <v>15.9390697387845</v>
+      </c>
+      <c r="C59">
+        <v>51.972170860519903</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60">
+        <v>31.285599186768799</v>
+      </c>
+      <c r="C60">
+        <v>37.520533971605197</v>
+      </c>
+      <c r="D60" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61">
+        <v>17.492590788015502</v>
+      </c>
+      <c r="C61">
+        <v>42.672913634251401</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62">
+        <v>19.105101674335302</v>
+      </c>
+      <c r="C62">
+        <v>43.798022378159096</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63">
+        <v>24.967763593252101</v>
+      </c>
+      <c r="C63">
+        <v>39.603397035794202</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64">
+        <v>22.407248227179501</v>
+      </c>
+      <c r="C64">
+        <v>38.1852309403818</v>
+      </c>
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64">
+        <v>14.2736</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66">
+        <v>49.442821432658199</v>
+      </c>
+      <c r="C66">
+        <v>37.939442749485899</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67">
+        <v>54.129459801485801</v>
+      </c>
+      <c r="C67">
+        <v>32.9072395561017</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68">
+        <v>57.946036778560703</v>
+      </c>
+      <c r="C68">
+        <v>36.718968554221902</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69">
+        <v>52.551957643016401</v>
+      </c>
+      <c r="C69">
+        <v>40.293876658129797</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B70">
+        <v>46.833569643669499</v>
+      </c>
+      <c r="C70">
+        <v>38.616925541429801</v>
+      </c>
+      <c r="D70" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71">
+        <v>56.389213194155403</v>
+      </c>
+      <c r="C71">
+        <v>27.371609496951301</v>
+      </c>
+      <c r="D71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72">
+        <v>46.746951404140297</v>
+      </c>
+      <c r="C72">
+        <v>29.150656427415399</v>
+      </c>
+      <c r="D72" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73">
+        <v>47.999406556587601</v>
+      </c>
+      <c r="C73">
+        <v>30.9284857033837</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74">
+        <v>53.0376851192364</v>
+      </c>
+      <c r="C74">
+        <v>26.672137423633799</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75">
+        <v>50.483440509278203</v>
+      </c>
+      <c r="C75">
+        <v>24.858796003070001</v>
+      </c>
+      <c r="D75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77">
+        <v>49.515628055574503</v>
+      </c>
+      <c r="C77">
+        <v>38.069836389263401</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78">
+        <v>55.022747106561901</v>
+      </c>
+      <c r="C78">
+        <v>32.803828369523899</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>58.115156968154402</v>
+      </c>
+      <c r="C79">
+        <v>36.812318442568703</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80">
+        <v>52.604039179984298</v>
+      </c>
+      <c r="C80">
+        <v>41.006215390358598</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81">
+        <v>46.831504870653397</v>
+      </c>
+      <c r="C81">
+        <v>38.488154853993798</v>
+      </c>
+      <c r="D81" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82">
+        <v>56.862790017769399</v>
+      </c>
+      <c r="C82">
+        <v>27.1500649319334</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83">
+        <v>46.818315133180299</v>
+      </c>
+      <c r="C83">
+        <v>28.838268038404301</v>
+      </c>
+      <c r="D83" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84">
+        <v>48.530662384139802</v>
+      </c>
+      <c r="C84">
+        <v>30.428467225865202</v>
+      </c>
+      <c r="D84" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85">
+        <v>53.221917571050298</v>
+      </c>
+      <c r="C85">
+        <v>26.415136622843999</v>
+      </c>
+      <c r="D85" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86">
+        <v>50.329363748321697</v>
+      </c>
+      <c r="C86">
+        <v>24.9620063898574</v>
+      </c>
+      <c r="D86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88">
+        <v>53.984644418664097</v>
+      </c>
+      <c r="C88">
+        <v>32.921131484599101</v>
+      </c>
+      <c r="D88" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89">
+        <v>60.9463987220295</v>
+      </c>
+      <c r="C89">
+        <v>25.940402743051202</v>
+      </c>
+      <c r="D89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90">
+        <v>65.214674169308196</v>
+      </c>
+      <c r="C90">
+        <v>27.6172583881275</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91">
+        <v>59.205588991080397</v>
+      </c>
+      <c r="C91">
+        <v>35.037476188758497</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92">
+        <v>44.909350845329399</v>
+      </c>
+      <c r="C92">
+        <v>39.218638661426397</v>
+      </c>
+      <c r="D92" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93">
+        <v>58.366418363549499</v>
+      </c>
+      <c r="C93">
+        <v>25.8923695064993</v>
+      </c>
+      <c r="D93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94">
+        <v>45.656437742964798</v>
+      </c>
+      <c r="C94">
+        <v>29.261364409462001</v>
+      </c>
+      <c r="D94" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B95">
+        <v>46.671702248429703</v>
+      </c>
+      <c r="C95">
+        <v>31.2259695150724</v>
+      </c>
+      <c r="D95" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B96">
+        <v>53.002093360166199</v>
+      </c>
+      <c r="C96">
+        <v>27.115006493862101</v>
+      </c>
+      <c r="D96" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B97">
+        <v>49.352867910798402</v>
+      </c>
+      <c r="C97">
+        <v>25.832633783943301</v>
+      </c>
+      <c r="D97" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99">
+        <v>53.568982586262102</v>
+      </c>
+      <c r="C99">
+        <v>32.709819641865899</v>
+      </c>
+      <c r="D99" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100">
+        <v>60.759584006742202</v>
+      </c>
+      <c r="C100">
+        <v>26.412804231665699</v>
+      </c>
+      <c r="D100" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101">
+        <v>65.066986353043802</v>
+      </c>
+      <c r="C101">
+        <v>29.1290574226168</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102">
+        <v>56.690249300666899</v>
+      </c>
+      <c r="C102">
+        <v>37.134037248500299</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103">
+        <v>45.240144694777598</v>
+      </c>
+      <c r="C103">
+        <v>29.4345940568804</v>
+      </c>
+      <c r="D103" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B104">
+        <v>46.763043007947999</v>
+      </c>
+      <c r="C104">
+        <v>31.130675699945201</v>
+      </c>
+      <c r="D104" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105">
+        <v>51.4379661501548</v>
+      </c>
+      <c r="C105">
+        <v>27.889389823301201</v>
+      </c>
+      <c r="D105" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B106">
+        <v>49.109135541484697</v>
+      </c>
+      <c r="C106">
+        <v>26.0122832140285</v>
+      </c>
+      <c r="D106" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B107">
+        <v>44.185532846653203</v>
+      </c>
+      <c r="C107">
+        <v>39.709648916227302</v>
+      </c>
+      <c r="D107" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B108">
+        <v>59.322477748676803</v>
+      </c>
+      <c r="C108">
+        <v>24.847357087708499</v>
+      </c>
+      <c r="D108" t="s">
+        <v>5</v>
+      </c>
+      <c r="E108">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110">
+        <v>54.292081433148503</v>
+      </c>
+      <c r="C110">
+        <v>34.154240980285898</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B111">
+        <v>59.287470094799403</v>
+      </c>
+      <c r="C111">
+        <v>28.7254423390415</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112">
+        <v>64.272110130137705</v>
+      </c>
+      <c r="C112">
+        <v>31.522055805493601</v>
+      </c>
+      <c r="D112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113">
+        <v>56.763476339691898</v>
+      </c>
+      <c r="C113">
+        <v>37.795531231799302</v>
+      </c>
+      <c r="D113" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114">
+        <v>47.051299777637801</v>
+      </c>
+      <c r="C114">
+        <v>38.685627301650598</v>
+      </c>
+      <c r="D114" t="s">
+        <v>5</v>
+      </c>
+      <c r="E114">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115">
+        <v>57.422671342990697</v>
+      </c>
+      <c r="C115">
+        <v>26.087786695086901</v>
+      </c>
+      <c r="D115" t="s">
+        <v>5</v>
+      </c>
+      <c r="E115">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B116">
+        <v>46.453793153520202</v>
+      </c>
+      <c r="C116">
+        <v>30.015444196233599</v>
+      </c>
+      <c r="D116" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117">
+        <v>47.875158480886597</v>
+      </c>
+      <c r="C117">
+        <v>31.717970930321201</v>
+      </c>
+      <c r="D117" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118">
+        <v>51.989187485269099</v>
+      </c>
+      <c r="C118">
+        <v>27.876254896364401</v>
+      </c>
+      <c r="D118" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B119">
+        <v>49.328776949615097</v>
+      </c>
+      <c r="C119">
+        <v>26.403588369102</v>
+      </c>
+      <c r="D119" t="s">
+        <v>10</v>
+      </c>
+      <c r="E119">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121">
+        <v>59.886140880710599</v>
+      </c>
+      <c r="C121">
+        <v>28.895097634406302</v>
+      </c>
+      <c r="D121" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B122">
+        <v>54.150135542677297</v>
+      </c>
+      <c r="C122">
+        <v>34.669014713243698</v>
+      </c>
+      <c r="D122" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B123">
+        <v>57.0641232720643</v>
+      </c>
+      <c r="C123">
+        <v>37.789099875303897</v>
+      </c>
+      <c r="D123" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124">
+        <v>63.8115508729556</v>
+      </c>
+      <c r="C124">
+        <v>31.155009994966601</v>
+      </c>
+      <c r="D124" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B125">
+        <v>45.824569291530501</v>
+      </c>
+      <c r="C125">
+        <v>39.434671267113799</v>
+      </c>
+      <c r="D125" t="s">
+        <v>5</v>
+      </c>
+      <c r="E125">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126">
+        <v>57.8167214328776</v>
+      </c>
+      <c r="C126">
+        <v>26.356114960665099</v>
+      </c>
+      <c r="D126" t="s">
+        <v>5</v>
+      </c>
+      <c r="E126">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127">
+        <v>45.989018323007102</v>
+      </c>
+      <c r="C127">
+        <v>30.906025265279101</v>
+      </c>
+      <c r="D127" t="s">
+        <v>10</v>
+      </c>
+      <c r="E127">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B128">
+        <v>47.839132104754903</v>
+      </c>
+      <c r="C128">
+        <v>32.060802668472299</v>
+      </c>
+      <c r="D128" t="s">
+        <v>10</v>
+      </c>
+      <c r="E128">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129">
+        <v>54.169826891759399</v>
+      </c>
+      <c r="C129">
+        <v>27.411024045316999</v>
+      </c>
+      <c r="D129" t="s">
+        <v>10</v>
+      </c>
+      <c r="E129">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B130">
+        <v>50.379556028115999</v>
+      </c>
+      <c r="C130">
+        <v>26.112153314053799</v>
+      </c>
+      <c r="D130" t="s">
+        <v>10</v>
+      </c>
+      <c r="E130">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B132">
+        <v>59.548297048140299</v>
+      </c>
+      <c r="C132">
+        <v>28.3642167580078</v>
+      </c>
+      <c r="D132" t="s">
+        <v>6</v>
+      </c>
+      <c r="E132">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B133">
+        <v>53.591455932818299</v>
+      </c>
+      <c r="C133">
+        <v>33.746120419643297</v>
+      </c>
+      <c r="D133" t="s">
+        <v>6</v>
+      </c>
+      <c r="E133">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B134">
+        <v>56.695134542022302</v>
+      </c>
+      <c r="C134">
+        <v>38.0435140756829</v>
+      </c>
+      <c r="D134" t="s">
+        <v>6</v>
+      </c>
+      <c r="E134">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B135">
+        <v>63.460019447420201</v>
+      </c>
+      <c r="C135">
+        <v>30.878468502531099</v>
+      </c>
+      <c r="D135" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B136">
+        <v>45.761544430391098</v>
+      </c>
+      <c r="C136">
+        <v>39.352695920484599</v>
+      </c>
+      <c r="D136" t="s">
+        <v>5</v>
+      </c>
+      <c r="E136">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B137">
+        <v>58.218881083261699</v>
+      </c>
+      <c r="C137">
+        <v>26.205981420851401</v>
+      </c>
+      <c r="D137" t="s">
+        <v>5</v>
+      </c>
+      <c r="E137">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B138">
+        <v>45.229070443411402</v>
+      </c>
+      <c r="C138">
+        <v>31.127052649200799</v>
+      </c>
+      <c r="D138" t="s">
+        <v>10</v>
+      </c>
+      <c r="E138">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B139">
+        <v>47.070616361109799</v>
+      </c>
+      <c r="C139">
+        <v>32.712752672313698</v>
+      </c>
+      <c r="D139" t="s">
+        <v>10</v>
+      </c>
+      <c r="E139">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B140">
+        <v>53.080628302099903</v>
+      </c>
+      <c r="C140">
+        <v>27.4639002569909</v>
+      </c>
+      <c r="D140" t="s">
+        <v>10</v>
+      </c>
+      <c r="E140">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B141">
+        <v>50.3213800367961</v>
+      </c>
+      <c r="C141">
+        <v>25.875880936323998</v>
+      </c>
+      <c r="D141" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141">
+        <v>11.754099999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>